<commit_message>
Fix handling of land cover crosstabs with new transition coding
</commit_message>
<xml_diff>
--- a/te_algorithms/data/summary_table_ld_sdg.xlsx
+++ b/te_algorithms/data/summary_table_ld_sdg.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\azvoleff\Code\LandDegradation\trends.earth-prais-prep\docker\summary_worker\trends.earth-algorithms\te_algorithms\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29584ADD-4F90-47EA-954A-9D189C41DFDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44993D27-3EFB-4E94-9C22-A096125DA209}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -156,9 +156,6 @@
     <t>Other lands</t>
   </si>
   <si>
-    <t>* For the SDG indicator, areas are considered to be improved if they have "Improving" productivity, to be stable if they have "stable" productivity, and to be "degraded" if they are classified as "stressed", in "moderate decline" or "declining".</t>
-  </si>
-  <si>
     <t>Area of land with declining productivity by type of land cover transition (sq. km)</t>
   </si>
   <si>
@@ -241,6 +238,9 @@
   </si>
   <si>
     <t>h</t>
+  </si>
+  <si>
+    <t>* For the SDG indicator, areas are considered to be improved if they have "Improving" productivity, to be stable if they have "stable" or "stressed" productivity, and to be "degraded" if they are classified as in "moderate decline" or "declining".</t>
   </si>
 </sst>
 </file>
@@ -1071,7 +1071,9 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1589,7 +1591,7 @@
     </row>
     <row r="3" spans="1:10" s="50" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="132" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B3" s="134"/>
       <c r="C3" s="134"/>
@@ -1681,9 +1683,9 @@
     </row>
     <row r="11" spans="1:10" s="50" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="133" t="s">
-        <v>40</v>
-      </c>
-      <c r="B11" s="135"/>
+        <v>68</v>
+      </c>
+      <c r="B11" s="134"/>
       <c r="C11" s="135"/>
       <c r="D11" s="135"/>
       <c r="E11" s="135"/>
@@ -1691,7 +1693,7 @@
       <c r="G11" s="135"/>
       <c r="H11" s="135"/>
       <c r="I11" s="135"/>
-      <c r="J11" s="135"/>
+      <c r="J11" s="136"/>
     </row>
     <row r="12" spans="1:10" s="50" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="63"/>
@@ -1707,7 +1709,7 @@
     </row>
     <row r="13" spans="1:10" s="93" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="114" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B13" s="114"/>
       <c r="C13" s="114"/>
@@ -1722,7 +1724,7 @@
     <row r="14" spans="1:10" s="93" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="1"/>
       <c r="C14" s="100" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J14" s="99"/>
     </row>
@@ -1756,7 +1758,7 @@
     </row>
     <row r="16" spans="1:10" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="96" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B16" s="57" t="s">
         <v>16</v>
@@ -1927,7 +1929,7 @@
     </row>
     <row r="25" spans="1:10" s="93" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="113" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B25" s="113"/>
       <c r="C25" s="113"/>
@@ -1941,7 +1943,7 @@
     </row>
     <row r="26" spans="1:10" s="93" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C26" s="100" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J26" s="99"/>
     </row>
@@ -1974,7 +1976,7 @@
     </row>
     <row r="28" spans="1:10" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="96" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B28" s="57" t="s">
         <v>16</v>
@@ -2145,7 +2147,7 @@
     </row>
     <row r="37" spans="1:10" s="93" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="110" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B37" s="111"/>
       <c r="C37" s="111"/>
@@ -2160,13 +2162,13 @@
     <row r="38" spans="1:10" s="93" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B38" s="1"/>
       <c r="C38" s="100" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J38" s="99"/>
     </row>
     <row r="39" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="92" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B39" s="92"/>
       <c r="C39" s="59" t="s">
@@ -2196,7 +2198,7 @@
     </row>
     <row r="40" spans="1:10" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="96" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B40" s="57" t="s">
         <v>16</v>
@@ -2367,7 +2369,7 @@
     </row>
     <row r="49" spans="1:10" s="93" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="107" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B49" s="108"/>
       <c r="C49" s="108"/>
@@ -2382,7 +2384,7 @@
     <row r="50" spans="1:10" s="93" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B50" s="1"/>
       <c r="C50" s="100" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J50" s="99"/>
     </row>
@@ -2416,7 +2418,7 @@
     </row>
     <row r="52" spans="1:10" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="96" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B52" s="57" t="s">
         <v>16</v>
@@ -2587,7 +2589,7 @@
     </row>
     <row r="61" spans="1:10" s="93" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="104" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B61" s="105"/>
       <c r="C61" s="105"/>
@@ -2602,7 +2604,7 @@
     <row r="62" spans="1:10" s="93" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B62" s="1"/>
       <c r="C62" s="100" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J62" s="99"/>
     </row>
@@ -2636,7 +2638,7 @@
     </row>
     <row r="64" spans="1:10" s="50" customFormat="1" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="96" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B64" s="57" t="s">
         <v>16</v>
@@ -2807,7 +2809,7 @@
     </row>
     <row r="73" spans="1:10" s="93" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="101" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B73" s="102"/>
       <c r="C73" s="102"/>
@@ -2822,7 +2824,7 @@
     <row r="74" spans="1:10" s="93" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B74" s="1"/>
       <c r="C74" s="100" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J74" s="99"/>
     </row>
@@ -2856,7 +2858,7 @@
     </row>
     <row r="76" spans="1:10" s="50" customFormat="1" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="96" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B76" s="57" t="s">
         <v>16</v>
@@ -3157,7 +3159,7 @@
     <row r="11" spans="1:10" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4"/>
       <c r="F11" s="27" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G11" s="31" t="e">
         <f>#REF!/G22</f>
@@ -3169,7 +3171,7 @@
     </row>
     <row r="13" spans="1:10" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="122" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B13" s="122"/>
       <c r="C13" s="122"/>
@@ -3188,19 +3190,19 @@
       <c r="A15" s="120"/>
       <c r="B15" s="120"/>
       <c r="C15" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="D15" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="E15" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="D15" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="E15" s="17" t="s">
+      <c r="F15" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="G15" s="17" t="s">
         <v>59</v>
-      </c>
-      <c r="F15" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="G15" s="17" t="s">
-        <v>60</v>
       </c>
       <c r="H15" s="120"/>
       <c r="I15" s="120"/>
@@ -3354,13 +3356,13 @@
     </row>
     <row r="24" spans="1:10" s="93" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="115" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="25" spans="1:10" s="93" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="1"/>
       <c r="C25" s="97" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3389,7 +3391,7 @@
     </row>
     <row r="27" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="98" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B27" s="117" t="s">
         <v>16</v>
@@ -3487,7 +3489,7 @@
     </row>
     <row r="34" spans="1:10" s="38" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="121" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B34" s="124"/>
       <c r="C34" s="124"/>
@@ -3659,10 +3661,10 @@
       <c r="A13" s="120"/>
       <c r="B13" s="120"/>
       <c r="C13" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E13" s="18" t="s">
         <v>13</v>
@@ -3870,10 +3872,7 @@
         <f>SUM(D14:D20)</f>
         <v>0</v>
       </c>
-      <c r="E21" s="25">
-        <f>SUM(E14:E20)</f>
-        <v>0</v>
-      </c>
+      <c r="E21" s="25"/>
       <c r="F21" s="22"/>
       <c r="G21" s="120"/>
       <c r="H21" s="120"/>
@@ -3901,7 +3900,7 @@
     <row r="24" spans="1:10" s="93" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="1"/>
       <c r="C24" s="100" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J24" s="123"/>
     </row>
@@ -3935,7 +3934,7 @@
     </row>
     <row r="26" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="96" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B26" s="57" t="s">
         <v>16</v>
@@ -4106,9 +4105,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{418A0AC8-B454-4329-A17B-534BF9D05BAA}">
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E52" sqref="E52"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4122,7 +4119,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="64" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B1" s="65"/>
       <c r="C1" s="65"/>
@@ -4148,7 +4145,7 @@
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="132" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B3" s="134"/>
       <c r="C3" s="134"/>
@@ -4165,16 +4162,16 @@
       <c r="B4" s="62"/>
       <c r="C4" s="62"/>
       <c r="D4" s="71" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E4" s="90" t="s">
         <v>38</v>
       </c>
       <c r="F4" s="91" t="s">
+        <v>50</v>
+      </c>
+      <c r="G4" s="61" t="s">
         <v>51</v>
-      </c>
-      <c r="G4" s="61" t="s">
-        <v>52</v>
       </c>
       <c r="I4" s="62"/>
       <c r="J4" s="62"/>
@@ -4208,7 +4205,7 @@
       <c r="A6" s="63"/>
       <c r="B6" s="62"/>
       <c r="C6" s="67" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D6" s="72">
         <f>'SDG 15.3.1'!F6</f>
@@ -4230,7 +4227,7 @@
       <c r="A7" s="63"/>
       <c r="B7" s="62"/>
       <c r="C7" s="67" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D7" s="70">
         <f>'SDG 15.3.1'!F8</f>
@@ -4252,7 +4249,7 @@
       <c r="A8" s="63"/>
       <c r="B8" s="62"/>
       <c r="C8" s="67" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D8" s="74">
         <f>'SDG 15.3.1'!F8</f>
@@ -4274,7 +4271,7 @@
       <c r="A9" s="63"/>
       <c r="B9" s="62"/>
       <c r="C9" s="67" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D9" s="73">
         <f>'SDG 15.3.1'!F9</f>

</xml_diff>

<commit_message>
Ensure water is correctly excluded from soc tabulations
</commit_message>
<xml_diff>
--- a/te_algorithms/data/summary_table_ld_sdg.xlsx
+++ b/te_algorithms/data/summary_table_ld_sdg.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\azvoleff\Code\LandDegradation\trends.earth-prais-prep\docker\summary_worker\trends.earth-algorithms\te_algorithms\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44993D27-3EFB-4E94-9C22-A096125DA209}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95DB8B43-9971-412E-949D-F3A55BF60EBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6825" yWindow="5145" windowWidth="28800" windowHeight="15225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SDG 15.3.1" sheetId="5" r:id="rId1"/>
@@ -703,7 +703,7 @@
     <xf numFmtId="43" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="140">
+  <cellXfs count="133">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -920,42 +920,6 @@
     <xf numFmtId="10" fontId="9" fillId="9" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="9" fillId="8" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="9" fillId="8" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="4" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="4" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="9" fillId="13" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="9" fillId="13" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="9" fillId="9" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="9" fillId="9" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1082,6 +1046,21 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="15" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="9" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="9" fillId="13" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="9" fillId="9" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1444,18 +1423,18 @@
       <c r="A2" s="4"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="132" t="s">
+      <c r="A3" s="120" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="132"/>
-      <c r="C3" s="132"/>
-      <c r="D3" s="132"/>
-      <c r="E3" s="132"/>
-      <c r="F3" s="132"/>
-      <c r="G3" s="132"/>
-      <c r="H3" s="132"/>
-      <c r="I3" s="132"/>
-      <c r="J3" s="132"/>
+      <c r="B3" s="120"/>
+      <c r="C3" s="120"/>
+      <c r="D3" s="120"/>
+      <c r="E3" s="120"/>
+      <c r="F3" s="120"/>
+      <c r="G3" s="120"/>
+      <c r="H3" s="120"/>
+      <c r="I3" s="120"/>
+      <c r="J3" s="120"/>
     </row>
     <row r="4" spans="1:10" s="39" customFormat="1" ht="30.75" x14ac:dyDescent="0.3">
       <c r="A4" s="41"/>
@@ -1538,18 +1517,18 @@
       <c r="A10" s="4"/>
     </row>
     <row r="11" spans="1:10" s="37" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="133" t="s">
+      <c r="A11" s="121" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="133"/>
-      <c r="C11" s="133"/>
-      <c r="D11" s="133"/>
-      <c r="E11" s="133"/>
-      <c r="F11" s="133"/>
-      <c r="G11" s="133"/>
-      <c r="H11" s="133"/>
-      <c r="I11" s="133"/>
-      <c r="J11" s="133"/>
+      <c r="B11" s="121"/>
+      <c r="C11" s="121"/>
+      <c r="D11" s="121"/>
+      <c r="E11" s="121"/>
+      <c r="F11" s="121"/>
+      <c r="G11" s="121"/>
+      <c r="H11" s="121"/>
+      <c r="I11" s="121"/>
+      <c r="J11" s="121"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="33" t="s">
@@ -1590,18 +1569,18 @@
       <c r="A2" s="4"/>
     </row>
     <row r="3" spans="1:10" s="50" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="132" t="s">
+      <c r="A3" s="120" t="s">
         <v>46</v>
       </c>
-      <c r="B3" s="134"/>
-      <c r="C3" s="134"/>
-      <c r="D3" s="134"/>
-      <c r="E3" s="134"/>
-      <c r="F3" s="134"/>
-      <c r="G3" s="134"/>
-      <c r="H3" s="134"/>
-      <c r="I3" s="134"/>
-      <c r="J3" s="134"/>
+      <c r="B3" s="122"/>
+      <c r="C3" s="122"/>
+      <c r="D3" s="122"/>
+      <c r="E3" s="122"/>
+      <c r="F3" s="122"/>
+      <c r="G3" s="122"/>
+      <c r="H3" s="122"/>
+      <c r="I3" s="122"/>
+      <c r="J3" s="122"/>
     </row>
     <row r="4" spans="1:10" ht="30.75" x14ac:dyDescent="0.3">
       <c r="A4" s="4"/>
@@ -1682,55 +1661,55 @@
       <c r="J10" s="49"/>
     </row>
     <row r="11" spans="1:10" s="50" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="133" t="s">
+      <c r="A11" s="121" t="s">
         <v>68</v>
       </c>
-      <c r="B11" s="134"/>
-      <c r="C11" s="135"/>
-      <c r="D11" s="135"/>
-      <c r="E11" s="135"/>
-      <c r="F11" s="135"/>
-      <c r="G11" s="135"/>
-      <c r="H11" s="135"/>
-      <c r="I11" s="135"/>
-      <c r="J11" s="136"/>
+      <c r="B11" s="122"/>
+      <c r="C11" s="123"/>
+      <c r="D11" s="123"/>
+      <c r="E11" s="123"/>
+      <c r="F11" s="123"/>
+      <c r="G11" s="123"/>
+      <c r="H11" s="123"/>
+      <c r="I11" s="123"/>
+      <c r="J11" s="124"/>
     </row>
     <row r="12" spans="1:10" s="50" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="63"/>
-      <c r="B12" s="92"/>
-      <c r="C12" s="93"/>
-      <c r="D12" s="93"/>
-      <c r="E12" s="93"/>
-      <c r="F12" s="93"/>
-      <c r="G12" s="93"/>
-      <c r="H12" s="93"/>
-      <c r="I12" s="93"/>
-      <c r="J12" s="94"/>
-    </row>
-    <row r="13" spans="1:10" s="93" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="114" t="s">
+      <c r="B12" s="80"/>
+      <c r="C12" s="81"/>
+      <c r="D12" s="81"/>
+      <c r="E12" s="81"/>
+      <c r="F12" s="81"/>
+      <c r="G12" s="81"/>
+      <c r="H12" s="81"/>
+      <c r="I12" s="81"/>
+      <c r="J12" s="82"/>
+    </row>
+    <row r="13" spans="1:10" s="81" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="102" t="s">
         <v>43</v>
       </c>
-      <c r="B13" s="114"/>
-      <c r="C13" s="114"/>
-      <c r="D13" s="114"/>
-      <c r="E13" s="114"/>
-      <c r="F13" s="114"/>
-      <c r="G13" s="114"/>
-      <c r="H13" s="114"/>
-      <c r="I13" s="114"/>
-      <c r="J13" s="114"/>
-    </row>
-    <row r="14" spans="1:10" s="93" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="102"/>
+      <c r="C13" s="102"/>
+      <c r="D13" s="102"/>
+      <c r="E13" s="102"/>
+      <c r="F13" s="102"/>
+      <c r="G13" s="102"/>
+      <c r="H13" s="102"/>
+      <c r="I13" s="102"/>
+      <c r="J13" s="102"/>
+    </row>
+    <row r="14" spans="1:10" s="81" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="1"/>
-      <c r="C14" s="100" t="s">
+      <c r="C14" s="88" t="s">
         <v>62</v>
       </c>
-      <c r="J14" s="99"/>
+      <c r="J14" s="87"/>
     </row>
     <row r="15" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="92"/>
-      <c r="B15" s="92"/>
+      <c r="A15" s="80"/>
+      <c r="B15" s="80"/>
       <c r="C15" s="60" t="s">
         <v>16</v>
       </c>
@@ -1752,12 +1731,12 @@
       <c r="I15" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="J15" s="94" t="s">
+      <c r="J15" s="82" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="96" t="s">
+      <c r="A16" s="84" t="s">
         <v>56</v>
       </c>
       <c r="B16" s="57" t="s">
@@ -1776,7 +1755,7 @@
       </c>
     </row>
     <row r="17" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="95"/>
+      <c r="A17" s="83"/>
       <c r="B17" s="2" t="s">
         <v>4</v>
       </c>
@@ -1793,7 +1772,7 @@
       </c>
     </row>
     <row r="18" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="95"/>
+      <c r="A18" s="83"/>
       <c r="B18" s="2" t="s">
         <v>5</v>
       </c>
@@ -1810,7 +1789,7 @@
       </c>
     </row>
     <row r="19" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="95"/>
+      <c r="A19" s="83"/>
       <c r="B19" s="2" t="s">
         <v>6</v>
       </c>
@@ -1827,7 +1806,7 @@
       </c>
     </row>
     <row r="20" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="95"/>
+      <c r="A20" s="83"/>
       <c r="B20" s="2" t="s">
         <v>7</v>
       </c>
@@ -1844,7 +1823,7 @@
       </c>
     </row>
     <row r="21" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="95"/>
+      <c r="A21" s="83"/>
       <c r="B21" s="2" t="s">
         <v>39</v>
       </c>
@@ -1861,7 +1840,7 @@
       </c>
     </row>
     <row r="22" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="95"/>
+      <c r="A22" s="83"/>
       <c r="B22" s="2" t="s">
         <v>8</v>
       </c>
@@ -1916,39 +1895,39 @@
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="92"/>
-      <c r="B24" s="92"/>
-      <c r="C24" s="93"/>
-      <c r="D24" s="93"/>
-      <c r="E24" s="93"/>
-      <c r="F24" s="93"/>
-      <c r="G24" s="93"/>
-      <c r="H24" s="93"/>
-      <c r="I24" s="93"/>
-      <c r="J24" s="94"/>
-    </row>
-    <row r="25" spans="1:10" s="93" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="113" t="s">
+      <c r="A24" s="80"/>
+      <c r="B24" s="80"/>
+      <c r="C24" s="81"/>
+      <c r="D24" s="81"/>
+      <c r="E24" s="81"/>
+      <c r="F24" s="81"/>
+      <c r="G24" s="81"/>
+      <c r="H24" s="81"/>
+      <c r="I24" s="81"/>
+      <c r="J24" s="82"/>
+    </row>
+    <row r="25" spans="1:10" s="81" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="101" t="s">
         <v>42</v>
       </c>
-      <c r="B25" s="113"/>
-      <c r="C25" s="113"/>
-      <c r="D25" s="113"/>
-      <c r="E25" s="113"/>
-      <c r="F25" s="113"/>
-      <c r="G25" s="113"/>
-      <c r="H25" s="113"/>
-      <c r="I25" s="113"/>
-      <c r="J25" s="113"/>
-    </row>
-    <row r="26" spans="1:10" s="93" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C26" s="100" t="s">
+      <c r="B25" s="101"/>
+      <c r="C25" s="101"/>
+      <c r="D25" s="101"/>
+      <c r="E25" s="101"/>
+      <c r="F25" s="101"/>
+      <c r="G25" s="101"/>
+      <c r="H25" s="101"/>
+      <c r="I25" s="101"/>
+      <c r="J25" s="101"/>
+    </row>
+    <row r="26" spans="1:10" s="81" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C26" s="88" t="s">
         <v>62</v>
       </c>
-      <c r="J26" s="99"/>
+      <c r="J26" s="87"/>
     </row>
     <row r="27" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="92"/>
+      <c r="A27" s="80"/>
       <c r="C27" s="59" t="s">
         <v>16</v>
       </c>
@@ -1970,12 +1949,12 @@
       <c r="I27" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="J27" s="94" t="s">
+      <c r="J27" s="82" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="96" t="s">
+      <c r="A28" s="84" t="s">
         <v>56</v>
       </c>
       <c r="B28" s="57" t="s">
@@ -1994,7 +1973,7 @@
       </c>
     </row>
     <row r="29" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="95"/>
+      <c r="A29" s="83"/>
       <c r="B29" s="2" t="s">
         <v>4</v>
       </c>
@@ -2011,7 +1990,7 @@
       </c>
     </row>
     <row r="30" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="95"/>
+      <c r="A30" s="83"/>
       <c r="B30" s="2" t="s">
         <v>5</v>
       </c>
@@ -2028,7 +2007,7 @@
       </c>
     </row>
     <row r="31" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="95"/>
+      <c r="A31" s="83"/>
       <c r="B31" s="2" t="s">
         <v>6</v>
       </c>
@@ -2045,7 +2024,7 @@
       </c>
     </row>
     <row r="32" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="95"/>
+      <c r="A32" s="83"/>
       <c r="B32" s="2" t="s">
         <v>7</v>
       </c>
@@ -2062,7 +2041,7 @@
       </c>
     </row>
     <row r="33" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="95"/>
+      <c r="A33" s="83"/>
       <c r="B33" s="2" t="s">
         <v>39</v>
       </c>
@@ -2079,7 +2058,7 @@
       </c>
     </row>
     <row r="34" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="95"/>
+      <c r="A34" s="83"/>
       <c r="B34" s="2" t="s">
         <v>8</v>
       </c>
@@ -2134,43 +2113,43 @@
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" s="92"/>
-      <c r="B36" s="92"/>
-      <c r="C36" s="93"/>
-      <c r="D36" s="93"/>
-      <c r="E36" s="93"/>
-      <c r="F36" s="93"/>
-      <c r="G36" s="93"/>
-      <c r="H36" s="93"/>
-      <c r="I36" s="93"/>
-      <c r="J36" s="94"/>
-    </row>
-    <row r="37" spans="1:10" s="93" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="110" t="s">
+      <c r="A36" s="80"/>
+      <c r="B36" s="80"/>
+      <c r="C36" s="81"/>
+      <c r="D36" s="81"/>
+      <c r="E36" s="81"/>
+      <c r="F36" s="81"/>
+      <c r="G36" s="81"/>
+      <c r="H36" s="81"/>
+      <c r="I36" s="81"/>
+      <c r="J36" s="82"/>
+    </row>
+    <row r="37" spans="1:10" s="81" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="98" t="s">
         <v>41</v>
       </c>
-      <c r="B37" s="111"/>
-      <c r="C37" s="111"/>
-      <c r="D37" s="111"/>
-      <c r="E37" s="111"/>
-      <c r="F37" s="111"/>
-      <c r="G37" s="111"/>
-      <c r="H37" s="111"/>
-      <c r="I37" s="111"/>
-      <c r="J37" s="112"/>
-    </row>
-    <row r="38" spans="1:10" s="93" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="99"/>
+      <c r="C37" s="99"/>
+      <c r="D37" s="99"/>
+      <c r="E37" s="99"/>
+      <c r="F37" s="99"/>
+      <c r="G37" s="99"/>
+      <c r="H37" s="99"/>
+      <c r="I37" s="99"/>
+      <c r="J37" s="100"/>
+    </row>
+    <row r="38" spans="1:10" s="81" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B38" s="1"/>
-      <c r="C38" s="100" t="s">
+      <c r="C38" s="88" t="s">
         <v>62</v>
       </c>
-      <c r="J38" s="99"/>
+      <c r="J38" s="87"/>
     </row>
     <row r="39" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39" s="92" t="s">
+      <c r="A39" s="80" t="s">
         <v>67</v>
       </c>
-      <c r="B39" s="92"/>
+      <c r="B39" s="80"/>
       <c r="C39" s="59" t="s">
         <v>16</v>
       </c>
@@ -2192,12 +2171,12 @@
       <c r="I39" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="J39" s="94" t="s">
+      <c r="J39" s="82" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="96" t="s">
+      <c r="A40" s="84" t="s">
         <v>56</v>
       </c>
       <c r="B40" s="57" t="s">
@@ -2216,7 +2195,7 @@
       </c>
     </row>
     <row r="41" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="95"/>
+      <c r="A41" s="83"/>
       <c r="B41" s="2" t="s">
         <v>4</v>
       </c>
@@ -2233,7 +2212,7 @@
       </c>
     </row>
     <row r="42" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="95"/>
+      <c r="A42" s="83"/>
       <c r="B42" s="2" t="s">
         <v>5</v>
       </c>
@@ -2250,7 +2229,7 @@
       </c>
     </row>
     <row r="43" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="95"/>
+      <c r="A43" s="83"/>
       <c r="B43" s="2" t="s">
         <v>6</v>
       </c>
@@ -2267,7 +2246,7 @@
       </c>
     </row>
     <row r="44" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="95"/>
+      <c r="A44" s="83"/>
       <c r="B44" s="2" t="s">
         <v>7</v>
       </c>
@@ -2284,7 +2263,7 @@
       </c>
     </row>
     <row r="45" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="95"/>
+      <c r="A45" s="83"/>
       <c r="B45" s="2" t="s">
         <v>39</v>
       </c>
@@ -2301,7 +2280,7 @@
       </c>
     </row>
     <row r="46" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="95"/>
+      <c r="A46" s="83"/>
       <c r="B46" s="2" t="s">
         <v>8</v>
       </c>
@@ -2356,41 +2335,41 @@
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A48" s="92"/>
-      <c r="B48" s="92"/>
-      <c r="C48" s="93"/>
-      <c r="D48" s="93"/>
-      <c r="E48" s="93"/>
-      <c r="F48" s="93"/>
-      <c r="G48" s="93"/>
-      <c r="H48" s="93"/>
-      <c r="I48" s="93"/>
-      <c r="J48" s="94"/>
-    </row>
-    <row r="49" spans="1:10" s="93" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="107" t="s">
+      <c r="A48" s="80"/>
+      <c r="B48" s="80"/>
+      <c r="C48" s="81"/>
+      <c r="D48" s="81"/>
+      <c r="E48" s="81"/>
+      <c r="F48" s="81"/>
+      <c r="G48" s="81"/>
+      <c r="H48" s="81"/>
+      <c r="I48" s="81"/>
+      <c r="J48" s="82"/>
+    </row>
+    <row r="49" spans="1:10" s="81" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="95" t="s">
         <v>44</v>
       </c>
-      <c r="B49" s="108"/>
-      <c r="C49" s="108"/>
-      <c r="D49" s="108"/>
-      <c r="E49" s="108"/>
-      <c r="F49" s="108"/>
-      <c r="G49" s="108"/>
-      <c r="H49" s="108"/>
-      <c r="I49" s="108"/>
-      <c r="J49" s="109"/>
-    </row>
-    <row r="50" spans="1:10" s="93" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B49" s="96"/>
+      <c r="C49" s="96"/>
+      <c r="D49" s="96"/>
+      <c r="E49" s="96"/>
+      <c r="F49" s="96"/>
+      <c r="G49" s="96"/>
+      <c r="H49" s="96"/>
+      <c r="I49" s="96"/>
+      <c r="J49" s="97"/>
+    </row>
+    <row r="50" spans="1:10" s="81" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B50" s="1"/>
-      <c r="C50" s="100" t="s">
+      <c r="C50" s="88" t="s">
         <v>62</v>
       </c>
-      <c r="J50" s="99"/>
+      <c r="J50" s="87"/>
     </row>
     <row r="51" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A51" s="92"/>
-      <c r="B51" s="92"/>
+      <c r="A51" s="80"/>
+      <c r="B51" s="80"/>
       <c r="C51" s="59" t="s">
         <v>16</v>
       </c>
@@ -2412,12 +2391,12 @@
       <c r="I51" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="J51" s="94" t="s">
+      <c r="J51" s="82" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="52" spans="1:10" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="96" t="s">
+      <c r="A52" s="84" t="s">
         <v>56</v>
       </c>
       <c r="B52" s="57" t="s">
@@ -2436,7 +2415,7 @@
       </c>
     </row>
     <row r="53" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="95"/>
+      <c r="A53" s="83"/>
       <c r="B53" s="2" t="s">
         <v>4</v>
       </c>
@@ -2453,7 +2432,7 @@
       </c>
     </row>
     <row r="54" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="95"/>
+      <c r="A54" s="83"/>
       <c r="B54" s="2" t="s">
         <v>5</v>
       </c>
@@ -2470,7 +2449,7 @@
       </c>
     </row>
     <row r="55" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="95"/>
+      <c r="A55" s="83"/>
       <c r="B55" s="2" t="s">
         <v>6</v>
       </c>
@@ -2487,7 +2466,7 @@
       </c>
     </row>
     <row r="56" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="95"/>
+      <c r="A56" s="83"/>
       <c r="B56" s="2" t="s">
         <v>7</v>
       </c>
@@ -2504,7 +2483,7 @@
       </c>
     </row>
     <row r="57" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="95"/>
+      <c r="A57" s="83"/>
       <c r="B57" s="2" t="s">
         <v>39</v>
       </c>
@@ -2521,7 +2500,7 @@
       </c>
     </row>
     <row r="58" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="95"/>
+      <c r="A58" s="83"/>
       <c r="B58" s="2" t="s">
         <v>8</v>
       </c>
@@ -2576,41 +2555,41 @@
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A60" s="92"/>
-      <c r="B60" s="92"/>
-      <c r="C60" s="93"/>
-      <c r="D60" s="93"/>
-      <c r="E60" s="93"/>
-      <c r="F60" s="93"/>
-      <c r="G60" s="93"/>
-      <c r="H60" s="93"/>
-      <c r="I60" s="93"/>
-      <c r="J60" s="94"/>
-    </row>
-    <row r="61" spans="1:10" s="93" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="104" t="s">
+      <c r="A60" s="80"/>
+      <c r="B60" s="80"/>
+      <c r="C60" s="81"/>
+      <c r="D60" s="81"/>
+      <c r="E60" s="81"/>
+      <c r="F60" s="81"/>
+      <c r="G60" s="81"/>
+      <c r="H60" s="81"/>
+      <c r="I60" s="81"/>
+      <c r="J60" s="82"/>
+    </row>
+    <row r="61" spans="1:10" s="81" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="92" t="s">
         <v>40</v>
       </c>
-      <c r="B61" s="105"/>
-      <c r="C61" s="105"/>
-      <c r="D61" s="105"/>
-      <c r="E61" s="105"/>
-      <c r="F61" s="105"/>
-      <c r="G61" s="105"/>
-      <c r="H61" s="105"/>
-      <c r="I61" s="105"/>
-      <c r="J61" s="106"/>
-    </row>
-    <row r="62" spans="1:10" s="93" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B61" s="93"/>
+      <c r="C61" s="93"/>
+      <c r="D61" s="93"/>
+      <c r="E61" s="93"/>
+      <c r="F61" s="93"/>
+      <c r="G61" s="93"/>
+      <c r="H61" s="93"/>
+      <c r="I61" s="93"/>
+      <c r="J61" s="94"/>
+    </row>
+    <row r="62" spans="1:10" s="81" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B62" s="1"/>
-      <c r="C62" s="100" t="s">
+      <c r="C62" s="88" t="s">
         <v>62</v>
       </c>
-      <c r="J62" s="99"/>
+      <c r="J62" s="87"/>
     </row>
     <row r="63" spans="1:10" s="50" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A63" s="92"/>
-      <c r="B63" s="92"/>
+      <c r="A63" s="80"/>
+      <c r="B63" s="80"/>
       <c r="C63" s="59" t="s">
         <v>16</v>
       </c>
@@ -2632,12 +2611,12 @@
       <c r="I63" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="J63" s="94" t="s">
+      <c r="J63" s="82" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="64" spans="1:10" s="50" customFormat="1" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="96" t="s">
+      <c r="A64" s="84" t="s">
         <v>56</v>
       </c>
       <c r="B64" s="57" t="s">
@@ -2656,7 +2635,7 @@
       </c>
     </row>
     <row r="65" spans="1:10" s="50" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="95"/>
+      <c r="A65" s="83"/>
       <c r="B65" s="2" t="s">
         <v>4</v>
       </c>
@@ -2673,7 +2652,7 @@
       </c>
     </row>
     <row r="66" spans="1:10" s="50" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="95"/>
+      <c r="A66" s="83"/>
       <c r="B66" s="2" t="s">
         <v>5</v>
       </c>
@@ -2690,7 +2669,7 @@
       </c>
     </row>
     <row r="67" spans="1:10" s="50" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="95"/>
+      <c r="A67" s="83"/>
       <c r="B67" s="2" t="s">
         <v>6</v>
       </c>
@@ -2707,7 +2686,7 @@
       </c>
     </row>
     <row r="68" spans="1:10" s="50" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="95"/>
+      <c r="A68" s="83"/>
       <c r="B68" s="2" t="s">
         <v>7</v>
       </c>
@@ -2724,7 +2703,7 @@
       </c>
     </row>
     <row r="69" spans="1:10" s="50" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="95"/>
+      <c r="A69" s="83"/>
       <c r="B69" s="2" t="s">
         <v>39</v>
       </c>
@@ -2741,7 +2720,7 @@
       </c>
     </row>
     <row r="70" spans="1:10" s="50" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="95"/>
+      <c r="A70" s="83"/>
       <c r="B70" s="2" t="s">
         <v>8</v>
       </c>
@@ -2796,41 +2775,41 @@
       </c>
     </row>
     <row r="72" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="92"/>
-      <c r="B72" s="92"/>
-      <c r="C72" s="93"/>
-      <c r="D72" s="93"/>
-      <c r="E72" s="93"/>
-      <c r="F72" s="93"/>
-      <c r="G72" s="93"/>
-      <c r="H72" s="93"/>
-      <c r="I72" s="93"/>
-      <c r="J72" s="94"/>
-    </row>
-    <row r="73" spans="1:10" s="93" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="101" t="s">
+      <c r="A72" s="80"/>
+      <c r="B72" s="80"/>
+      <c r="C72" s="81"/>
+      <c r="D72" s="81"/>
+      <c r="E72" s="81"/>
+      <c r="F72" s="81"/>
+      <c r="G72" s="81"/>
+      <c r="H72" s="81"/>
+      <c r="I72" s="81"/>
+      <c r="J72" s="82"/>
+    </row>
+    <row r="73" spans="1:10" s="81" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="89" t="s">
         <v>45</v>
       </c>
-      <c r="B73" s="102"/>
-      <c r="C73" s="102"/>
-      <c r="D73" s="102"/>
-      <c r="E73" s="102"/>
-      <c r="F73" s="102"/>
-      <c r="G73" s="102"/>
-      <c r="H73" s="102"/>
-      <c r="I73" s="102"/>
-      <c r="J73" s="103"/>
-    </row>
-    <row r="74" spans="1:10" s="93" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B73" s="90"/>
+      <c r="C73" s="90"/>
+      <c r="D73" s="90"/>
+      <c r="E73" s="90"/>
+      <c r="F73" s="90"/>
+      <c r="G73" s="90"/>
+      <c r="H73" s="90"/>
+      <c r="I73" s="90"/>
+      <c r="J73" s="91"/>
+    </row>
+    <row r="74" spans="1:10" s="81" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B74" s="1"/>
-      <c r="C74" s="100" t="s">
+      <c r="C74" s="88" t="s">
         <v>62</v>
       </c>
-      <c r="J74" s="99"/>
+      <c r="J74" s="87"/>
     </row>
     <row r="75" spans="1:10" s="50" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A75" s="92"/>
-      <c r="B75" s="92"/>
+      <c r="A75" s="80"/>
+      <c r="B75" s="80"/>
       <c r="C75" s="59" t="s">
         <v>16</v>
       </c>
@@ -2852,12 +2831,12 @@
       <c r="I75" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="J75" s="94" t="s">
+      <c r="J75" s="82" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="76" spans="1:10" s="50" customFormat="1" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="96" t="s">
+      <c r="A76" s="84" t="s">
         <v>56</v>
       </c>
       <c r="B76" s="57" t="s">
@@ -2876,7 +2855,7 @@
       </c>
     </row>
     <row r="77" spans="1:10" s="50" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="95"/>
+      <c r="A77" s="83"/>
       <c r="B77" s="2" t="s">
         <v>4</v>
       </c>
@@ -2893,7 +2872,7 @@
       </c>
     </row>
     <row r="78" spans="1:10" s="50" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="95"/>
+      <c r="A78" s="83"/>
       <c r="B78" s="2" t="s">
         <v>5</v>
       </c>
@@ -2910,7 +2889,7 @@
       </c>
     </row>
     <row r="79" spans="1:10" s="50" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="95"/>
+      <c r="A79" s="83"/>
       <c r="B79" s="2" t="s">
         <v>6</v>
       </c>
@@ -2927,7 +2906,7 @@
       </c>
     </row>
     <row r="80" spans="1:10" s="50" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="95"/>
+      <c r="A80" s="83"/>
       <c r="B80" s="2" t="s">
         <v>7</v>
       </c>
@@ -2944,7 +2923,7 @@
       </c>
     </row>
     <row r="81" spans="1:10" s="50" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="95"/>
+      <c r="A81" s="83"/>
       <c r="B81" s="2" t="s">
         <v>39</v>
       </c>
@@ -2961,7 +2940,7 @@
       </c>
     </row>
     <row r="82" spans="1:10" s="50" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="95"/>
+      <c r="A82" s="83"/>
       <c r="B82" s="2" t="s">
         <v>8</v>
       </c>
@@ -3048,18 +3027,18 @@
       <c r="A2" s="4"/>
     </row>
     <row r="3" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="132" t="s">
+      <c r="A3" s="120" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="134"/>
-      <c r="C3" s="134"/>
-      <c r="D3" s="134"/>
-      <c r="E3" s="134"/>
-      <c r="F3" s="134"/>
-      <c r="G3" s="134"/>
-      <c r="H3" s="134"/>
-      <c r="I3" s="134"/>
-      <c r="J3" s="134"/>
+      <c r="B3" s="122"/>
+      <c r="C3" s="122"/>
+      <c r="D3" s="122"/>
+      <c r="E3" s="122"/>
+      <c r="F3" s="122"/>
+      <c r="G3" s="122"/>
+      <c r="H3" s="122"/>
+      <c r="I3" s="122"/>
+      <c r="J3" s="122"/>
     </row>
     <row r="4" spans="1:10" ht="30.75" x14ac:dyDescent="0.3">
       <c r="A4" s="4"/>
@@ -3170,25 +3149,25 @@
       <c r="A12" s="4"/>
     </row>
     <row r="13" spans="1:10" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="122" t="s">
+      <c r="A13" s="110" t="s">
         <v>66</v>
       </c>
-      <c r="B13" s="122"/>
-      <c r="C13" s="122"/>
-      <c r="D13" s="122"/>
-      <c r="E13" s="122"/>
-      <c r="F13" s="122"/>
-      <c r="G13" s="122"/>
-      <c r="H13" s="122"/>
-      <c r="I13" s="122"/>
-      <c r="J13" s="122"/>
+      <c r="B13" s="110"/>
+      <c r="C13" s="110"/>
+      <c r="D13" s="110"/>
+      <c r="E13" s="110"/>
+      <c r="F13" s="110"/>
+      <c r="G13" s="110"/>
+      <c r="H13" s="110"/>
+      <c r="I13" s="110"/>
+      <c r="J13" s="110"/>
     </row>
     <row r="14" spans="1:10" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4"/>
     </row>
     <row r="15" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="120"/>
-      <c r="B15" s="120"/>
+      <c r="A15" s="108"/>
+      <c r="B15" s="108"/>
       <c r="C15" s="17" t="s">
         <v>57</v>
       </c>
@@ -3204,11 +3183,11 @@
       <c r="G15" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="H15" s="120"/>
-      <c r="I15" s="120"/>
+      <c r="H15" s="108"/>
+      <c r="I15" s="108"/>
     </row>
     <row r="16" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="125"/>
+      <c r="A16" s="113"/>
       <c r="B16" s="57" t="s">
         <v>16</v>
       </c>
@@ -3223,11 +3202,11 @@
       <c r="E16" s="26"/>
       <c r="F16" s="26"/>
       <c r="G16" s="26"/>
-      <c r="H16" s="120"/>
-      <c r="I16" s="120"/>
+      <c r="H16" s="108"/>
+      <c r="I16" s="108"/>
     </row>
     <row r="17" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="95"/>
+      <c r="A17" s="83"/>
       <c r="B17" s="2" t="s">
         <v>4</v>
       </c>
@@ -3242,11 +3221,11 @@
       <c r="E17" s="26"/>
       <c r="F17" s="26"/>
       <c r="G17" s="26"/>
-      <c r="H17" s="120"/>
-      <c r="I17" s="120"/>
+      <c r="H17" s="108"/>
+      <c r="I17" s="108"/>
     </row>
     <row r="18" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="95"/>
+      <c r="A18" s="83"/>
       <c r="B18" s="2" t="s">
         <v>5</v>
       </c>
@@ -3261,11 +3240,11 @@
       <c r="E18" s="26"/>
       <c r="F18" s="26"/>
       <c r="G18" s="26"/>
-      <c r="H18" s="120"/>
-      <c r="I18" s="120"/>
+      <c r="H18" s="108"/>
+      <c r="I18" s="108"/>
     </row>
     <row r="19" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="95"/>
+      <c r="A19" s="83"/>
       <c r="B19" s="2" t="s">
         <v>6</v>
       </c>
@@ -3280,11 +3259,11 @@
       <c r="E19" s="26"/>
       <c r="F19" s="26"/>
       <c r="G19" s="26"/>
-      <c r="H19" s="120"/>
-      <c r="I19" s="120"/>
+      <c r="H19" s="108"/>
+      <c r="I19" s="108"/>
     </row>
     <row r="20" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="95"/>
+      <c r="A20" s="83"/>
       <c r="B20" s="2" t="s">
         <v>7</v>
       </c>
@@ -3299,11 +3278,11 @@
       <c r="E20" s="26"/>
       <c r="F20" s="26"/>
       <c r="G20" s="26"/>
-      <c r="H20" s="120"/>
-      <c r="I20" s="120"/>
+      <c r="H20" s="108"/>
+      <c r="I20" s="108"/>
     </row>
     <row r="21" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="95"/>
+      <c r="A21" s="83"/>
       <c r="B21" s="2" t="s">
         <v>39</v>
       </c>
@@ -3318,12 +3297,12 @@
       <c r="E21" s="26"/>
       <c r="F21" s="26"/>
       <c r="G21" s="26"/>
-      <c r="H21" s="120"/>
-      <c r="I21" s="120"/>
+      <c r="H21" s="108"/>
+      <c r="I21" s="108"/>
     </row>
     <row r="22" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="9"/>
-      <c r="B22" s="120"/>
+      <c r="B22" s="108"/>
       <c r="C22" s="25"/>
       <c r="D22" s="6" t="s">
         <v>9</v>
@@ -3340,34 +3319,34 @@
         <f>SUM(G16:G21)</f>
         <v>0</v>
       </c>
-      <c r="H22" s="120"/>
-      <c r="I22" s="120"/>
+      <c r="H22" s="108"/>
+      <c r="I22" s="108"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="120"/>
-      <c r="B23" s="120"/>
-      <c r="C23" s="120"/>
-      <c r="D23" s="120"/>
-      <c r="E23" s="120"/>
-      <c r="F23" s="120"/>
-      <c r="G23" s="120"/>
-      <c r="H23" s="120"/>
-      <c r="I23" s="120"/>
-    </row>
-    <row r="24" spans="1:10" s="93" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="115" t="s">
+      <c r="A23" s="108"/>
+      <c r="B23" s="108"/>
+      <c r="C23" s="108"/>
+      <c r="D23" s="108"/>
+      <c r="E23" s="108"/>
+      <c r="F23" s="108"/>
+      <c r="G23" s="108"/>
+      <c r="H23" s="108"/>
+      <c r="I23" s="108"/>
+    </row>
+    <row r="24" spans="1:10" s="81" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="103" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="25" spans="1:10" s="93" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" s="81" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="1"/>
-      <c r="C25" s="97" t="s">
+      <c r="C25" s="85" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="120"/>
-      <c r="B26" s="93"/>
+      <c r="A26" s="108"/>
+      <c r="B26" s="81"/>
       <c r="C26" s="32" t="s">
         <v>16</v>
       </c>
@@ -3386,120 +3365,120 @@
       <c r="H26" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="I26" s="126"/>
-      <c r="J26" s="127"/>
+      <c r="I26" s="114"/>
+      <c r="J26" s="115"/>
     </row>
     <row r="27" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="98" t="s">
+      <c r="A27" s="86" t="s">
         <v>56</v>
       </c>
-      <c r="B27" s="117" t="s">
+      <c r="B27" s="105" t="s">
         <v>16</v>
       </c>
-      <c r="C27" s="118"/>
-      <c r="D27" s="118"/>
-      <c r="E27" s="118"/>
-      <c r="F27" s="118"/>
-      <c r="G27" s="118"/>
-      <c r="H27" s="118"/>
-      <c r="I27" s="131"/>
-      <c r="J27" s="127"/>
+      <c r="C27" s="106"/>
+      <c r="D27" s="106"/>
+      <c r="E27" s="106"/>
+      <c r="F27" s="106"/>
+      <c r="G27" s="106"/>
+      <c r="H27" s="106"/>
+      <c r="I27" s="119"/>
+      <c r="J27" s="115"/>
     </row>
     <row r="28" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="95"/>
-      <c r="B28" s="119" t="s">
+      <c r="A28" s="83"/>
+      <c r="B28" s="107" t="s">
         <v>4</v>
       </c>
-      <c r="C28" s="118"/>
-      <c r="D28" s="118"/>
-      <c r="E28" s="118"/>
-      <c r="F28" s="118"/>
-      <c r="G28" s="118"/>
-      <c r="H28" s="118"/>
-      <c r="I28" s="131"/>
-      <c r="J28" s="127"/>
+      <c r="C28" s="106"/>
+      <c r="D28" s="106"/>
+      <c r="E28" s="106"/>
+      <c r="F28" s="106"/>
+      <c r="G28" s="106"/>
+      <c r="H28" s="106"/>
+      <c r="I28" s="119"/>
+      <c r="J28" s="115"/>
     </row>
     <row r="29" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="95"/>
-      <c r="B29" s="119" t="s">
+      <c r="A29" s="83"/>
+      <c r="B29" s="107" t="s">
         <v>5</v>
       </c>
-      <c r="C29" s="118"/>
-      <c r="D29" s="118"/>
-      <c r="E29" s="118"/>
-      <c r="F29" s="118"/>
-      <c r="G29" s="118"/>
-      <c r="H29" s="118"/>
-      <c r="I29" s="131"/>
-      <c r="J29" s="127"/>
+      <c r="C29" s="106"/>
+      <c r="D29" s="106"/>
+      <c r="E29" s="106"/>
+      <c r="F29" s="106"/>
+      <c r="G29" s="106"/>
+      <c r="H29" s="106"/>
+      <c r="I29" s="119"/>
+      <c r="J29" s="115"/>
     </row>
     <row r="30" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="95"/>
-      <c r="B30" s="119" t="s">
+      <c r="A30" s="83"/>
+      <c r="B30" s="107" t="s">
         <v>6</v>
       </c>
-      <c r="C30" s="118"/>
-      <c r="D30" s="118"/>
-      <c r="E30" s="118"/>
-      <c r="F30" s="118"/>
-      <c r="G30" s="118"/>
-      <c r="H30" s="118"/>
-      <c r="I30" s="131"/>
-      <c r="J30" s="127"/>
+      <c r="C30" s="106"/>
+      <c r="D30" s="106"/>
+      <c r="E30" s="106"/>
+      <c r="F30" s="106"/>
+      <c r="G30" s="106"/>
+      <c r="H30" s="106"/>
+      <c r="I30" s="119"/>
+      <c r="J30" s="115"/>
     </row>
     <row r="31" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="95"/>
-      <c r="B31" s="119" t="s">
+      <c r="A31" s="83"/>
+      <c r="B31" s="107" t="s">
         <v>7</v>
       </c>
-      <c r="C31" s="118"/>
-      <c r="D31" s="118"/>
-      <c r="E31" s="118"/>
-      <c r="F31" s="118"/>
-      <c r="G31" s="118"/>
-      <c r="H31" s="118"/>
-      <c r="I31" s="131"/>
-      <c r="J31" s="127"/>
+      <c r="C31" s="106"/>
+      <c r="D31" s="106"/>
+      <c r="E31" s="106"/>
+      <c r="F31" s="106"/>
+      <c r="G31" s="106"/>
+      <c r="H31" s="106"/>
+      <c r="I31" s="119"/>
+      <c r="J31" s="115"/>
     </row>
     <row r="32" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="95"/>
-      <c r="B32" s="119" t="s">
+      <c r="A32" s="83"/>
+      <c r="B32" s="107" t="s">
         <v>39</v>
       </c>
-      <c r="C32" s="118"/>
-      <c r="D32" s="118"/>
-      <c r="E32" s="118"/>
-      <c r="F32" s="118"/>
-      <c r="G32" s="118"/>
-      <c r="H32" s="118"/>
-      <c r="I32" s="131"/>
-      <c r="J32" s="127"/>
+      <c r="C32" s="106"/>
+      <c r="D32" s="106"/>
+      <c r="E32" s="106"/>
+      <c r="F32" s="106"/>
+      <c r="G32" s="106"/>
+      <c r="H32" s="106"/>
+      <c r="I32" s="119"/>
+      <c r="J32" s="115"/>
     </row>
     <row r="33" spans="1:10" s="38" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="8"/>
-      <c r="B33" s="123"/>
-      <c r="C33" s="130"/>
-      <c r="D33" s="130"/>
-      <c r="E33" s="130"/>
-      <c r="F33" s="130"/>
-      <c r="G33" s="130"/>
-      <c r="H33" s="130"/>
-      <c r="I33" s="128"/>
-      <c r="J33" s="128"/>
+      <c r="B33" s="111"/>
+      <c r="C33" s="118"/>
+      <c r="D33" s="118"/>
+      <c r="E33" s="118"/>
+      <c r="F33" s="118"/>
+      <c r="G33" s="118"/>
+      <c r="H33" s="118"/>
+      <c r="I33" s="116"/>
+      <c r="J33" s="116"/>
     </row>
     <row r="34" spans="1:10" s="38" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="121" t="s">
+      <c r="A34" s="109" t="s">
         <v>63</v>
       </c>
-      <c r="B34" s="124"/>
-      <c r="C34" s="124"/>
-      <c r="D34" s="124"/>
-      <c r="E34" s="124"/>
-      <c r="F34" s="124"/>
-      <c r="G34" s="124"/>
-      <c r="H34" s="124"/>
-      <c r="I34" s="129"/>
-      <c r="J34" s="129"/>
+      <c r="B34" s="112"/>
+      <c r="C34" s="112"/>
+      <c r="D34" s="112"/>
+      <c r="E34" s="112"/>
+      <c r="F34" s="112"/>
+      <c r="G34" s="112"/>
+      <c r="H34" s="112"/>
+      <c r="I34" s="117"/>
+      <c r="J34" s="117"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3535,18 +3514,18 @@
       <c r="A2" s="4"/>
     </row>
     <row r="3" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="132" t="s">
+      <c r="A3" s="120" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="134"/>
-      <c r="C3" s="134"/>
-      <c r="D3" s="134"/>
-      <c r="E3" s="134"/>
-      <c r="F3" s="134"/>
-      <c r="G3" s="134"/>
-      <c r="H3" s="134"/>
-      <c r="I3" s="134"/>
-      <c r="J3" s="136"/>
+      <c r="B3" s="122"/>
+      <c r="C3" s="122"/>
+      <c r="D3" s="122"/>
+      <c r="E3" s="122"/>
+      <c r="F3" s="122"/>
+      <c r="G3" s="122"/>
+      <c r="H3" s="122"/>
+      <c r="I3" s="122"/>
+      <c r="J3" s="124"/>
     </row>
     <row r="4" spans="1:10" ht="30.75" x14ac:dyDescent="0.3">
       <c r="A4" s="4"/>
@@ -3640,26 +3619,26 @@
       <c r="J10" s="34"/>
     </row>
     <row r="11" spans="1:10" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="137" t="s">
+      <c r="A11" s="125" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="138"/>
-      <c r="C11" s="138"/>
-      <c r="D11" s="138"/>
-      <c r="E11" s="138"/>
-      <c r="F11" s="138"/>
-      <c r="G11" s="138"/>
-      <c r="H11" s="138"/>
-      <c r="I11" s="138"/>
-      <c r="J11" s="139"/>
+      <c r="B11" s="126"/>
+      <c r="C11" s="126"/>
+      <c r="D11" s="126"/>
+      <c r="E11" s="126"/>
+      <c r="F11" s="126"/>
+      <c r="G11" s="126"/>
+      <c r="H11" s="126"/>
+      <c r="I11" s="126"/>
+      <c r="J11" s="127"/>
     </row>
     <row r="12" spans="1:10" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>
       <c r="J12" s="34"/>
     </row>
     <row r="13" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="120"/>
-      <c r="B13" s="120"/>
+      <c r="A13" s="108"/>
+      <c r="B13" s="108"/>
       <c r="C13" s="17" t="s">
         <v>58</v>
       </c>
@@ -3672,13 +3651,13 @@
       <c r="F13" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="G13" s="120"/>
-      <c r="H13" s="120"/>
-      <c r="I13" s="120"/>
-      <c r="J13" s="123"/>
+      <c r="G13" s="108"/>
+      <c r="H13" s="108"/>
+      <c r="I13" s="108"/>
+      <c r="J13" s="111"/>
     </row>
     <row r="14" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="125"/>
+      <c r="A14" s="113"/>
       <c r="B14" s="57" t="s">
         <v>16</v>
       </c>
@@ -3698,13 +3677,13 @@
         <f t="shared" ref="F14:F20" si="3">(D14-C14)/C14</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G14" s="120"/>
-      <c r="H14" s="120"/>
-      <c r="I14" s="120"/>
-      <c r="J14" s="123"/>
+      <c r="G14" s="108"/>
+      <c r="H14" s="108"/>
+      <c r="I14" s="108"/>
+      <c r="J14" s="111"/>
     </row>
     <row r="15" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="125"/>
+      <c r="A15" s="113"/>
       <c r="B15" s="2" t="s">
         <v>4</v>
       </c>
@@ -3724,13 +3703,13 @@
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G15" s="120"/>
-      <c r="H15" s="120"/>
-      <c r="I15" s="120"/>
-      <c r="J15" s="123"/>
+      <c r="G15" s="108"/>
+      <c r="H15" s="108"/>
+      <c r="I15" s="108"/>
+      <c r="J15" s="111"/>
     </row>
     <row r="16" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="125"/>
+      <c r="A16" s="113"/>
       <c r="B16" s="2" t="s">
         <v>5</v>
       </c>
@@ -3750,13 +3729,13 @@
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G16" s="120"/>
-      <c r="H16" s="120"/>
-      <c r="I16" s="120"/>
-      <c r="J16" s="123"/>
+      <c r="G16" s="108"/>
+      <c r="H16" s="108"/>
+      <c r="I16" s="108"/>
+      <c r="J16" s="111"/>
     </row>
     <row r="17" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="125"/>
+      <c r="A17" s="113"/>
       <c r="B17" s="2" t="s">
         <v>6</v>
       </c>
@@ -3776,13 +3755,13 @@
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G17" s="120"/>
-      <c r="H17" s="120"/>
-      <c r="I17" s="120"/>
-      <c r="J17" s="123"/>
+      <c r="G17" s="108"/>
+      <c r="H17" s="108"/>
+      <c r="I17" s="108"/>
+      <c r="J17" s="111"/>
     </row>
     <row r="18" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="125"/>
+      <c r="A18" s="113"/>
       <c r="B18" s="2" t="s">
         <v>7</v>
       </c>
@@ -3802,13 +3781,13 @@
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G18" s="120"/>
-      <c r="H18" s="120"/>
-      <c r="I18" s="120"/>
-      <c r="J18" s="123"/>
+      <c r="G18" s="108"/>
+      <c r="H18" s="108"/>
+      <c r="I18" s="108"/>
+      <c r="J18" s="111"/>
     </row>
     <row r="19" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="125"/>
+      <c r="A19" s="113"/>
       <c r="B19" s="2" t="s">
         <v>39</v>
       </c>
@@ -3828,13 +3807,13 @@
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G19" s="120"/>
-      <c r="H19" s="120"/>
-      <c r="I19" s="120"/>
-      <c r="J19" s="123"/>
+      <c r="G19" s="108"/>
+      <c r="H19" s="108"/>
+      <c r="I19" s="108"/>
+      <c r="J19" s="111"/>
     </row>
     <row r="20" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="125"/>
+      <c r="A20" s="113"/>
       <c r="B20" s="2" t="s">
         <v>8</v>
       </c>
@@ -3854,10 +3833,10 @@
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G20" s="120"/>
-      <c r="H20" s="120"/>
-      <c r="I20" s="120"/>
-      <c r="J20" s="123"/>
+      <c r="G20" s="108"/>
+      <c r="H20" s="108"/>
+      <c r="I20" s="108"/>
+      <c r="J20" s="111"/>
     </row>
     <row r="21" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="9"/>
@@ -3874,39 +3853,39 @@
       </c>
       <c r="E21" s="25"/>
       <c r="F21" s="22"/>
-      <c r="G21" s="120"/>
-      <c r="H21" s="120"/>
-      <c r="I21" s="120"/>
-      <c r="J21" s="123"/>
+      <c r="G21" s="108"/>
+      <c r="H21" s="108"/>
+      <c r="I21" s="108"/>
+      <c r="J21" s="111"/>
     </row>
     <row r="22" spans="1:10" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="63"/>
       <c r="B22" s="6"/>
       <c r="C22" s="19"/>
       <c r="D22" s="19"/>
-      <c r="E22" s="120"/>
-      <c r="F22" s="120"/>
-      <c r="G22" s="120"/>
-      <c r="H22" s="120"/>
-      <c r="I22" s="120"/>
-      <c r="J22" s="123"/>
-    </row>
-    <row r="23" spans="1:10" s="93" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="116" t="s">
+      <c r="E22" s="108"/>
+      <c r="F22" s="108"/>
+      <c r="G22" s="108"/>
+      <c r="H22" s="108"/>
+      <c r="I22" s="108"/>
+      <c r="J22" s="111"/>
+    </row>
+    <row r="23" spans="1:10" s="81" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="104" t="s">
         <v>15</v>
       </c>
-      <c r="J23" s="123"/>
-    </row>
-    <row r="24" spans="1:10" s="93" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J23" s="111"/>
+    </row>
+    <row r="24" spans="1:10" s="81" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="1"/>
-      <c r="C24" s="100" t="s">
+      <c r="C24" s="88" t="s">
         <v>62</v>
       </c>
-      <c r="J24" s="123"/>
+      <c r="J24" s="111"/>
     </row>
     <row r="25" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="120"/>
-      <c r="B25" s="120"/>
+      <c r="A25" s="108"/>
+      <c r="B25" s="108"/>
       <c r="C25" s="58" t="s">
         <v>16</v>
       </c>
@@ -3928,12 +3907,12 @@
       <c r="I25" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="J25" s="123" t="s">
+      <c r="J25" s="111" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="96" t="s">
+      <c r="A26" s="84" t="s">
         <v>56</v>
       </c>
       <c r="B26" s="57" t="s">
@@ -3952,7 +3931,7 @@
       </c>
     </row>
     <row r="27" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="95"/>
+      <c r="A27" s="83"/>
       <c r="B27" s="2" t="s">
         <v>4</v>
       </c>
@@ -3969,7 +3948,7 @@
       </c>
     </row>
     <row r="28" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="95"/>
+      <c r="A28" s="83"/>
       <c r="B28" s="2" t="s">
         <v>5</v>
       </c>
@@ -3986,7 +3965,7 @@
       </c>
     </row>
     <row r="29" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="95"/>
+      <c r="A29" s="83"/>
       <c r="B29" s="2" t="s">
         <v>6</v>
       </c>
@@ -4003,7 +3982,7 @@
       </c>
     </row>
     <row r="30" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="95"/>
+      <c r="A30" s="83"/>
       <c r="B30" s="2" t="s">
         <v>7</v>
       </c>
@@ -4020,7 +3999,7 @@
       </c>
     </row>
     <row r="31" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="95"/>
+      <c r="A31" s="83"/>
       <c r="B31" s="2" t="s">
         <v>39</v>
       </c>
@@ -4037,7 +4016,7 @@
       </c>
     </row>
     <row r="32" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="95"/>
+      <c r="A32" s="83"/>
       <c r="B32" s="2" t="s">
         <v>8</v>
       </c>
@@ -4144,18 +4123,18 @@
       <c r="J2" s="62"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="132" t="s">
+      <c r="A3" s="120" t="s">
         <v>48</v>
       </c>
-      <c r="B3" s="134"/>
-      <c r="C3" s="134"/>
-      <c r="D3" s="134"/>
-      <c r="E3" s="134"/>
-      <c r="F3" s="134"/>
-      <c r="G3" s="134"/>
-      <c r="H3" s="134"/>
-      <c r="I3" s="134"/>
-      <c r="J3" s="136"/>
+      <c r="B3" s="122"/>
+      <c r="C3" s="122"/>
+      <c r="D3" s="122"/>
+      <c r="E3" s="122"/>
+      <c r="F3" s="122"/>
+      <c r="G3" s="122"/>
+      <c r="H3" s="122"/>
+      <c r="I3" s="122"/>
+      <c r="J3" s="124"/>
     </row>
     <row r="4" spans="1:10" ht="41.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="63"/>
@@ -4164,10 +4143,10 @@
       <c r="D4" s="71" t="s">
         <v>49</v>
       </c>
-      <c r="E4" s="90" t="s">
+      <c r="E4" s="61" t="s">
         <v>38</v>
       </c>
-      <c r="F4" s="91" t="s">
+      <c r="F4" s="61" t="s">
         <v>50</v>
       </c>
       <c r="G4" s="61" t="s">
@@ -4186,11 +4165,11 @@
         <f>'SDG 15.3.1'!F5</f>
         <v>0</v>
       </c>
-      <c r="E5" s="80" t="e">
+      <c r="E5" s="75" t="e">
         <f>'SDG 15.3.1'!G5</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="F5" s="81">
+      <c r="F5" s="128">
         <f>SUM(F6:F9)</f>
         <v>0</v>
       </c>
@@ -4211,11 +4190,11 @@
         <f>'SDG 15.3.1'!F6</f>
         <v>0</v>
       </c>
-      <c r="E6" s="82" t="e">
+      <c r="E6" s="76" t="e">
         <f>'SDG 15.3.1'!G6</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="F6" s="83"/>
+      <c r="F6" s="129"/>
       <c r="G6" s="76" t="e">
         <f>F6/F$5</f>
         <v>#DIV/0!</v>
@@ -4233,11 +4212,11 @@
         <f>'SDG 15.3.1'!F8</f>
         <v>0</v>
       </c>
-      <c r="E7" s="84" t="e">
+      <c r="E7" s="77" t="e">
         <f>'SDG 15.3.1'!G7</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="F7" s="85"/>
+      <c r="F7" s="130"/>
       <c r="G7" s="77" t="e">
         <f>F7/F$5</f>
         <v>#DIV/0!</v>
@@ -4255,11 +4234,11 @@
         <f>'SDG 15.3.1'!F8</f>
         <v>0</v>
       </c>
-      <c r="E8" s="86" t="e">
+      <c r="E8" s="78" t="e">
         <f>'SDG 15.3.1'!G8</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="F8" s="87"/>
+      <c r="F8" s="131"/>
       <c r="G8" s="78" t="e">
         <f>F8/F$5</f>
         <v>#DIV/0!</v>
@@ -4277,11 +4256,11 @@
         <f>'SDG 15.3.1'!F9</f>
         <v>0</v>
       </c>
-      <c r="E9" s="88" t="e">
+      <c r="E9" s="79" t="e">
         <f>'SDG 15.3.1'!G9</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="F9" s="89"/>
+      <c r="F9" s="132"/>
       <c r="G9" s="79" t="e">
         <f>F9/F$5</f>
         <v>#DIV/0!</v>

</xml_diff>